<commit_message>
Actualizacion presuspuesto ABP sin completar
</commit_message>
<xml_diff>
--- a/Documentacion/Copia de Plantilla_Presupuesto_ABP_2016-17.xlsx
+++ b/Documentacion/Copia de Plantilla_Presupuesto_ABP_2016-17.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mis Cosas\Universidad\ABP\Repositorio\Estudio Rorschach\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="576" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="576" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Principal - ABP" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <definedName name="Graficos1" localSheetId="4">#REF!</definedName>
     <definedName name="Graficos1">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -3023,7 +3023,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -4863,12 +4863,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="145" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="44" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="45" xfId="145" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="11" borderId="46" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="145" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="13" borderId="1" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4880,15 +4889,6 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="14" borderId="1" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="44" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="45" xfId="145" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -7506,7 +7506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6:Q18"/>
     </sheetView>
   </sheetViews>
@@ -10691,7 +10691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
@@ -10704,32 +10704,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="266" t="s">
+      <c r="A1" s="261" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="266"/>
-      <c r="C1" s="266"/>
-      <c r="D1" s="266"/>
-      <c r="E1" s="266"/>
-      <c r="F1" s="266"/>
-      <c r="G1" s="266"/>
-      <c r="H1" s="266"/>
-      <c r="I1" s="266"/>
-      <c r="J1" s="266"/>
+      <c r="B1" s="261"/>
+      <c r="C1" s="261"/>
+      <c r="D1" s="261"/>
+      <c r="E1" s="261"/>
+      <c r="F1" s="261"/>
+      <c r="G1" s="261"/>
+      <c r="H1" s="261"/>
+      <c r="I1" s="261"/>
+      <c r="J1" s="261"/>
     </row>
     <row r="2" spans="1:10" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="267" t="s">
+      <c r="A2" s="262" t="s">
         <v>211</v>
       </c>
-      <c r="B2" s="267"/>
-      <c r="C2" s="267"/>
-      <c r="D2" s="267"/>
-      <c r="E2" s="267"/>
-      <c r="F2" s="267"/>
-      <c r="G2" s="267"/>
-      <c r="H2" s="267"/>
-      <c r="I2" s="267"/>
-      <c r="J2" s="267"/>
+      <c r="B2" s="262"/>
+      <c r="C2" s="262"/>
+      <c r="D2" s="262"/>
+      <c r="E2" s="262"/>
+      <c r="F2" s="262"/>
+      <c r="G2" s="262"/>
+      <c r="H2" s="262"/>
+      <c r="I2" s="262"/>
+      <c r="J2" s="262"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="67"/>
@@ -10744,20 +10744,20 @@
       <c r="J3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="20.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="268" t="s">
+      <c r="A4" s="263" t="s">
         <v>212</v>
       </c>
-      <c r="B4" s="268"/>
+      <c r="B4" s="263"/>
       <c r="C4" s="67"/>
-      <c r="D4" s="268" t="s">
+      <c r="D4" s="263" t="s">
         <v>213</v>
       </c>
-      <c r="E4" s="268"/>
-      <c r="F4" s="268"/>
-      <c r="G4" s="268"/>
-      <c r="H4" s="268"/>
-      <c r="I4" s="268"/>
-      <c r="J4" s="268"/>
+      <c r="E4" s="263"/>
+      <c r="F4" s="263"/>
+      <c r="G4" s="263"/>
+      <c r="H4" s="263"/>
+      <c r="I4" s="263"/>
+      <c r="J4" s="263"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="68" t="s">
@@ -10767,14 +10767,14 @@
         <v>215</v>
       </c>
       <c r="C5" s="67"/>
-      <c r="D5" s="261" t="s">
+      <c r="D5" s="260" t="s">
         <v>216</v>
       </c>
-      <c r="E5" s="261"/>
-      <c r="F5" s="261"/>
-      <c r="G5" s="261"/>
-      <c r="H5" s="261"/>
-      <c r="I5" s="261"/>
+      <c r="E5" s="260"/>
+      <c r="F5" s="260"/>
+      <c r="G5" s="260"/>
+      <c r="H5" s="260"/>
+      <c r="I5" s="260"/>
       <c r="J5" s="70">
         <f>'Principal - ABP'!G19</f>
         <v>6</v>
@@ -10788,14 +10788,14 @@
         <v>10</v>
       </c>
       <c r="C6" s="67"/>
-      <c r="D6" s="261" t="s">
+      <c r="D6" s="260" t="s">
         <v>218</v>
       </c>
-      <c r="E6" s="261"/>
-      <c r="F6" s="261"/>
-      <c r="G6" s="261"/>
-      <c r="H6" s="261"/>
-      <c r="I6" s="261"/>
+      <c r="E6" s="260"/>
+      <c r="F6" s="260"/>
+      <c r="G6" s="260"/>
+      <c r="H6" s="260"/>
+      <c r="I6" s="260"/>
       <c r="J6" s="72">
         <f>J5*B7</f>
         <v>660</v>
@@ -10809,14 +10809,14 @@
         <v>110</v>
       </c>
       <c r="C7" s="67"/>
-      <c r="D7" s="261" t="s">
+      <c r="D7" s="260" t="s">
         <v>220</v>
       </c>
-      <c r="E7" s="261"/>
-      <c r="F7" s="261"/>
-      <c r="G7" s="261"/>
-      <c r="H7" s="261"/>
-      <c r="I7" s="261"/>
+      <c r="E7" s="260"/>
+      <c r="F7" s="260"/>
+      <c r="G7" s="260"/>
+      <c r="H7" s="260"/>
+      <c r="I7" s="260"/>
       <c r="J7" s="73">
         <f>I13</f>
         <v>665</v>
@@ -10830,14 +10830,14 @@
         <v>30</v>
       </c>
       <c r="C8" s="67"/>
-      <c r="D8" s="261" t="s">
+      <c r="D8" s="260" t="s">
         <v>222</v>
       </c>
-      <c r="E8" s="261"/>
-      <c r="F8" s="261"/>
-      <c r="G8" s="261"/>
-      <c r="H8" s="261"/>
-      <c r="I8" s="261"/>
+      <c r="E8" s="260"/>
+      <c r="F8" s="260"/>
+      <c r="G8" s="260"/>
+      <c r="H8" s="260"/>
+      <c r="I8" s="260"/>
       <c r="J8" s="74">
         <f>ABS(J6-J7)/J6</f>
         <v>7.575757575757576E-3</v>
@@ -10852,14 +10852,14 @@
         <v>150</v>
       </c>
       <c r="C9" s="67"/>
-      <c r="D9" s="262" t="s">
+      <c r="D9" s="265" t="s">
         <v>223</v>
       </c>
-      <c r="E9" s="262"/>
-      <c r="F9" s="262"/>
-      <c r="G9" s="262"/>
-      <c r="H9" s="262"/>
-      <c r="I9" s="262"/>
+      <c r="E9" s="265"/>
+      <c r="F9" s="265"/>
+      <c r="G9" s="265"/>
+      <c r="H9" s="265"/>
+      <c r="I9" s="265"/>
       <c r="J9" s="77">
         <f>J13</f>
         <v>60.454545454545446</v>
@@ -10878,37 +10878,37 @@
       <c r="J10" s="67"/>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="263" t="s">
+      <c r="A11" s="266" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="263" t="s">
+      <c r="B11" s="266" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="263" t="s">
+      <c r="C11" s="266" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="264" t="s">
+      <c r="D11" s="267" t="s">
         <v>224</v>
       </c>
-      <c r="E11" s="265" t="s">
+      <c r="E11" s="268" t="s">
         <v>225</v>
       </c>
-      <c r="F11" s="264" t="s">
+      <c r="F11" s="267" t="s">
         <v>226</v>
       </c>
-      <c r="G11" s="264"/>
-      <c r="H11" s="264"/>
-      <c r="I11" s="265" t="s">
+      <c r="G11" s="267"/>
+      <c r="H11" s="267"/>
+      <c r="I11" s="268" t="s">
         <v>227</v>
       </c>
-      <c r="J11" s="265"/>
+      <c r="J11" s="268"/>
     </row>
     <row r="12" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="263"/>
-      <c r="B12" s="263"/>
-      <c r="C12" s="263"/>
-      <c r="D12" s="264"/>
-      <c r="E12" s="264"/>
+      <c r="A12" s="266"/>
+      <c r="B12" s="266"/>
+      <c r="C12" s="266"/>
+      <c r="D12" s="267"/>
+      <c r="E12" s="267"/>
       <c r="F12" s="78" t="s">
         <v>228</v>
       </c>
@@ -10926,14 +10926,14 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="260"/>
-      <c r="B13" s="260"/>
-      <c r="C13" s="260"/>
-      <c r="D13" s="260"/>
-      <c r="E13" s="260"/>
-      <c r="F13" s="260"/>
-      <c r="G13" s="260"/>
-      <c r="H13" s="260"/>
+      <c r="A13" s="264"/>
+      <c r="B13" s="264"/>
+      <c r="C13" s="264"/>
+      <c r="D13" s="264"/>
+      <c r="E13" s="264"/>
+      <c r="F13" s="264"/>
+      <c r="G13" s="264"/>
+      <c r="H13" s="264"/>
       <c r="I13" s="80">
         <f>SUM(I14:I49)</f>
         <v>665</v>
@@ -12042,12 +12042,6 @@
   </sheetData>
   <sheetProtection password="C894" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="17">
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:J4"/>
-    <mergeCell ref="D5:I5"/>
     <mergeCell ref="A13:H13"/>
     <mergeCell ref="D7:I7"/>
     <mergeCell ref="D8:I8"/>
@@ -12059,6 +12053,12 @@
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="I11:J11"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:J4"/>
+    <mergeCell ref="D5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="J8">
     <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
@@ -12086,8 +12086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12099,32 +12099,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="266" t="s">
+      <c r="A1" s="261" t="s">
         <v>315</v>
       </c>
-      <c r="B1" s="266"/>
-      <c r="C1" s="266"/>
-      <c r="D1" s="266"/>
-      <c r="E1" s="266"/>
-      <c r="F1" s="266"/>
-      <c r="G1" s="266"/>
-      <c r="H1" s="266"/>
-      <c r="I1" s="266"/>
-      <c r="J1" s="266"/>
+      <c r="B1" s="261"/>
+      <c r="C1" s="261"/>
+      <c r="D1" s="261"/>
+      <c r="E1" s="261"/>
+      <c r="F1" s="261"/>
+      <c r="G1" s="261"/>
+      <c r="H1" s="261"/>
+      <c r="I1" s="261"/>
+      <c r="J1" s="261"/>
     </row>
     <row r="2" spans="1:10" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="267" t="s">
+      <c r="A2" s="262" t="s">
         <v>211</v>
       </c>
-      <c r="B2" s="267"/>
-      <c r="C2" s="267"/>
-      <c r="D2" s="267"/>
-      <c r="E2" s="267"/>
-      <c r="F2" s="267"/>
-      <c r="G2" s="267"/>
-      <c r="H2" s="267"/>
-      <c r="I2" s="267"/>
-      <c r="J2" s="267"/>
+      <c r="B2" s="262"/>
+      <c r="C2" s="262"/>
+      <c r="D2" s="262"/>
+      <c r="E2" s="262"/>
+      <c r="F2" s="262"/>
+      <c r="G2" s="262"/>
+      <c r="H2" s="262"/>
+      <c r="I2" s="262"/>
+      <c r="J2" s="262"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="67"/>
@@ -12139,20 +12139,20 @@
       <c r="J3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="20.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="268" t="s">
+      <c r="A4" s="263" t="s">
         <v>212</v>
       </c>
-      <c r="B4" s="268"/>
+      <c r="B4" s="263"/>
       <c r="C4" s="67"/>
-      <c r="D4" s="268" t="s">
+      <c r="D4" s="263" t="s">
         <v>213</v>
       </c>
-      <c r="E4" s="268"/>
-      <c r="F4" s="268"/>
-      <c r="G4" s="268"/>
-      <c r="H4" s="268"/>
-      <c r="I4" s="268"/>
-      <c r="J4" s="268"/>
+      <c r="E4" s="263"/>
+      <c r="F4" s="263"/>
+      <c r="G4" s="263"/>
+      <c r="H4" s="263"/>
+      <c r="I4" s="263"/>
+      <c r="J4" s="263"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="68" t="s">
@@ -12162,14 +12162,14 @@
         <v>215</v>
       </c>
       <c r="C5" s="67"/>
-      <c r="D5" s="261" t="s">
+      <c r="D5" s="260" t="s">
         <v>216</v>
       </c>
-      <c r="E5" s="261"/>
-      <c r="F5" s="261"/>
-      <c r="G5" s="261"/>
-      <c r="H5" s="261"/>
-      <c r="I5" s="261"/>
+      <c r="E5" s="260"/>
+      <c r="F5" s="260"/>
+      <c r="G5" s="260"/>
+      <c r="H5" s="260"/>
+      <c r="I5" s="260"/>
       <c r="J5" s="70">
         <f>'Principal - ABP'!G19</f>
         <v>6</v>
@@ -12183,14 +12183,14 @@
         <v>10</v>
       </c>
       <c r="C6" s="67"/>
-      <c r="D6" s="261" t="s">
+      <c r="D6" s="260" t="s">
         <v>218</v>
       </c>
-      <c r="E6" s="261"/>
-      <c r="F6" s="261"/>
-      <c r="G6" s="261"/>
-      <c r="H6" s="261"/>
-      <c r="I6" s="261"/>
+      <c r="E6" s="260"/>
+      <c r="F6" s="260"/>
+      <c r="G6" s="260"/>
+      <c r="H6" s="260"/>
+      <c r="I6" s="260"/>
       <c r="J6" s="72">
         <f>J5*B7</f>
         <v>660</v>
@@ -12204,17 +12204,17 @@
         <v>110</v>
       </c>
       <c r="C7" s="67"/>
-      <c r="D7" s="261" t="s">
+      <c r="D7" s="260" t="s">
         <v>220</v>
       </c>
-      <c r="E7" s="261"/>
-      <c r="F7" s="261"/>
-      <c r="G7" s="261"/>
-      <c r="H7" s="261"/>
-      <c r="I7" s="261"/>
+      <c r="E7" s="260"/>
+      <c r="F7" s="260"/>
+      <c r="G7" s="260"/>
+      <c r="H7" s="260"/>
+      <c r="I7" s="260"/>
       <c r="J7" s="73">
         <f>I13</f>
-        <v>648</v>
+        <v>571</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12225,17 +12225,17 @@
         <v>30</v>
       </c>
       <c r="C8" s="67"/>
-      <c r="D8" s="261" t="s">
+      <c r="D8" s="260" t="s">
         <v>222</v>
       </c>
-      <c r="E8" s="261"/>
-      <c r="F8" s="261"/>
-      <c r="G8" s="261"/>
-      <c r="H8" s="261"/>
-      <c r="I8" s="261"/>
+      <c r="E8" s="260"/>
+      <c r="F8" s="260"/>
+      <c r="G8" s="260"/>
+      <c r="H8" s="260"/>
+      <c r="I8" s="260"/>
       <c r="J8" s="74">
         <f>ABS(J6-J7)/J6</f>
-        <v>1.8181818181818181E-2</v>
+        <v>0.13484848484848486</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
@@ -12247,17 +12247,17 @@
         <v>150</v>
       </c>
       <c r="C9" s="67"/>
-      <c r="D9" s="262" t="s">
+      <c r="D9" s="265" t="s">
         <v>223</v>
       </c>
-      <c r="E9" s="262"/>
-      <c r="F9" s="262"/>
-      <c r="G9" s="262"/>
-      <c r="H9" s="262"/>
-      <c r="I9" s="262"/>
+      <c r="E9" s="265"/>
+      <c r="F9" s="265"/>
+      <c r="G9" s="265"/>
+      <c r="H9" s="265"/>
+      <c r="I9" s="265"/>
       <c r="J9" s="77">
         <f>J13</f>
-        <v>58.909090909090928</v>
+        <v>51.909090909090928</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -12273,37 +12273,37 @@
       <c r="J10" s="67"/>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="263" t="s">
+      <c r="A11" s="266" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="263" t="s">
+      <c r="B11" s="266" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="263" t="s">
+      <c r="C11" s="266" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="264" t="s">
+      <c r="D11" s="267" t="s">
         <v>224</v>
       </c>
-      <c r="E11" s="265" t="s">
+      <c r="E11" s="268" t="s">
         <v>225</v>
       </c>
-      <c r="F11" s="264" t="s">
+      <c r="F11" s="267" t="s">
         <v>226</v>
       </c>
-      <c r="G11" s="264"/>
-      <c r="H11" s="264"/>
-      <c r="I11" s="265" t="s">
+      <c r="G11" s="267"/>
+      <c r="H11" s="267"/>
+      <c r="I11" s="268" t="s">
         <v>227</v>
       </c>
-      <c r="J11" s="265"/>
+      <c r="J11" s="268"/>
     </row>
     <row r="12" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="263"/>
-      <c r="B12" s="263"/>
-      <c r="C12" s="263"/>
-      <c r="D12" s="264"/>
-      <c r="E12" s="264"/>
+      <c r="A12" s="266"/>
+      <c r="B12" s="266"/>
+      <c r="C12" s="266"/>
+      <c r="D12" s="267"/>
+      <c r="E12" s="267"/>
       <c r="F12" s="78" t="s">
         <v>228</v>
       </c>
@@ -12321,21 +12321,21 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="260"/>
-      <c r="B13" s="260"/>
-      <c r="C13" s="260"/>
-      <c r="D13" s="260"/>
-      <c r="E13" s="260"/>
-      <c r="F13" s="260"/>
-      <c r="G13" s="260"/>
-      <c r="H13" s="260"/>
+      <c r="A13" s="264"/>
+      <c r="B13" s="264"/>
+      <c r="C13" s="264"/>
+      <c r="D13" s="264"/>
+      <c r="E13" s="264"/>
+      <c r="F13" s="264"/>
+      <c r="G13" s="264"/>
+      <c r="H13" s="264"/>
       <c r="I13" s="80">
         <f>SUM(I14:I48)</f>
-        <v>648</v>
+        <v>571</v>
       </c>
       <c r="J13" s="80">
         <f>SUM(J14:J48)</f>
-        <v>58.909090909090928</v>
+        <v>51.909090909090928</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -13073,9 +13073,7 @@
       <c r="D36" s="81" t="s">
         <v>369</v>
       </c>
-      <c r="E36" s="84">
-        <v>2</v>
-      </c>
+      <c r="E36" s="84"/>
       <c r="F36" s="85"/>
       <c r="G36" s="85">
         <v>5</v>
@@ -13084,12 +13082,10 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="I36" s="87">
-        <v>5</v>
-      </c>
+      <c r="I36" s="87"/>
       <c r="J36" s="88">
         <f t="shared" si="1"/>
-        <v>0.45454545454545459</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -13105,9 +13101,7 @@
       <c r="D37" s="81">
         <v>2</v>
       </c>
-      <c r="E37" s="92">
-        <v>2</v>
-      </c>
+      <c r="E37" s="92"/>
       <c r="F37" s="85">
         <v>5</v>
       </c>
@@ -13118,12 +13112,10 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="I37" s="87">
-        <v>55</v>
-      </c>
+      <c r="I37" s="87"/>
       <c r="J37" s="88">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -13237,9 +13229,7 @@
       <c r="D41" s="81" t="s">
         <v>374</v>
       </c>
-      <c r="E41" s="84">
-        <v>3</v>
-      </c>
+      <c r="E41" s="84"/>
       <c r="F41" s="85">
         <v>2</v>
       </c>
@@ -13250,12 +13240,10 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="I41" s="87">
-        <v>17</v>
-      </c>
+      <c r="I41" s="87"/>
       <c r="J41" s="88">
         <f t="shared" si="1"/>
-        <v>1.5454545454545454</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -13481,6 +13469,12 @@
   </sheetData>
   <sheetProtection password="C894" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="17">
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:J4"/>
+    <mergeCell ref="D5:I5"/>
     <mergeCell ref="A13:H13"/>
     <mergeCell ref="D7:I7"/>
     <mergeCell ref="D8:I8"/>
@@ -13492,12 +13486,6 @@
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="I11:J11"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:J4"/>
-    <mergeCell ref="D5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="J8">
     <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">

</xml_diff>